<commit_message>
updating bill of parts - tough not rigid plastic for jig parts
</commit_message>
<xml_diff>
--- a/Bill of Parts.xlsx
+++ b/Bill of Parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubCodeRepositories\SpikeGadgets_OpenEphys_Drive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Design Git Repos\SpikeGadgets_OpenEphys_Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="798">
   <si>
     <t>Jakob Voigts, Jonathan P. Newman, Matthew A. Wilson, Mark T. Harnett</t>
   </si>
@@ -2390,9 +2390,6 @@
     <t>DIY fabrication</t>
   </si>
   <si>
-    <t>Formlabs RIGID at 50-100 um</t>
-  </si>
-  <si>
     <t>formlabs clear at 50 um</t>
   </si>
   <si>
@@ -2402,18 +2399,12 @@
     <t>formlabs clear at 50 um layer height</t>
   </si>
   <si>
-    <t>Formlabs RIGID at 50-100 um layer height</t>
-  </si>
-  <si>
     <t>check dowel diameter… this may be for mouse</t>
   </si>
   <si>
     <t>actually really helpful</t>
   </si>
   <si>
-    <t>** when using rigid, be sure to cure correctly</t>
-  </si>
-  <si>
     <t>formlabs grey pro or black, or tough</t>
   </si>
   <si>
@@ -2424,6 +2415,12 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/91595A490/</t>
+  </si>
+  <si>
+    <t>Formlabs TOUGH at 50-100 um layer height</t>
+  </si>
+  <si>
+    <t>** when using tough, be sure to cure correctly</t>
   </si>
 </sst>
 </file>
@@ -2984,26 +2981,26 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="3" width="39.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="3" width="39.1796875" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.5703125" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="52.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.54296875" customWidth="1"/>
+    <col min="7" max="7" width="29.1796875" customWidth="1"/>
+    <col min="8" max="10" width="8.54296875" customWidth="1"/>
+    <col min="11" max="11" width="6.81640625" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="52.26953125" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -3011,7 +3008,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>89</v>
       </c>
@@ -3046,7 +3043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -3054,12 +3051,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>791</v>
+        <v>796</v>
       </c>
       <c r="D4" t="s">
         <v>139</v>
@@ -3077,12 +3074,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="D5" t="s">
         <v>139</v>
@@ -3100,12 +3097,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="D6" t="s">
         <v>140</v>
@@ -3123,12 +3120,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="D7" t="s">
         <v>140</v>
@@ -3146,12 +3143,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="D8" t="s">
         <v>140</v>
@@ -3169,12 +3166,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="D9" t="s">
         <v>140</v>
@@ -3192,17 +3189,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="28" t="s">
         <v>771</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>123</v>
@@ -3211,7 +3208,7 @@
         <v>72</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="G11" s="35" t="s">
         <v>772</v>
@@ -3235,7 +3232,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="28" t="s">
         <v>773</v>
       </c>
@@ -3269,12 +3266,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="28" t="s">
         <v>76</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>128</v>
@@ -3305,7 +3302,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="28" t="s">
         <v>764</v>
       </c>
@@ -3336,7 +3333,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="28" t="s">
         <v>765</v>
       </c>
@@ -3367,7 +3364,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -3375,20 +3372,20 @@
         <v>777</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
+        <v>788</v>
+      </c>
+      <c r="C19" t="s">
         <v>789</v>
       </c>
-      <c r="C19" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D20" t="s">
         <v>145</v>
@@ -3412,12 +3409,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>138</v>
       </c>
       <c r="C21" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="D21" t="s">
         <v>141</v>
@@ -3444,7 +3441,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -3476,7 +3473,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="6" t="s">
         <v>22</v>
       </c>
@@ -3517,7 +3514,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>148</v>
       </c>
@@ -3532,7 +3529,7 @@
         <v>30</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="I24" s="26"/>
       <c r="M24" s="40" t="s">
@@ -3543,7 +3540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="6" t="s">
         <v>38</v>
       </c>
@@ -3564,7 +3561,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>766</v>
       </c>
@@ -3584,7 +3581,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B27" s="42" t="s">
         <v>779</v>
       </c>
@@ -3593,17 +3590,17 @@
         <v>785</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="26" x14ac:dyDescent="0.35">
       <c r="B29" s="42" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="6" t="s">
         <v>48</v>
       </c>
@@ -3623,7 +3620,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="6" t="s">
         <v>50</v>
       </c>
@@ -3643,7 +3640,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="2:13" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" ht="43" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="8" t="s">
         <v>51</v>
       </c>
@@ -3663,7 +3660,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="6" t="s">
         <v>54</v>
       </c>
@@ -3683,7 +3680,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B36" s="42" t="s">
         <v>162</v>
       </c>
@@ -3711,12 +3708,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
         <v>770</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D43" t="s">
         <v>781</v>
       </c>
@@ -3730,7 +3727,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D44">
         <v>1</v>
       </c>
@@ -3746,7 +3743,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D45">
         <v>0.5</v>
       </c>
@@ -3762,7 +3759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D46">
         <v>0.25</v>
       </c>
@@ -3779,7 +3776,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D47">
         <v>0.125</v>
       </c>
@@ -3796,7 +3793,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
       <c r="D48">
         <v>0.1</v>
       </c>
@@ -3812,7 +3809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D49">
         <f>D48/2</f>
         <v>0.05</v>
@@ -3829,7 +3826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D50">
         <f>D49/2</f>
         <v>2.5000000000000001E-2</v>
@@ -3846,7 +3843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D51">
         <f>D50/2</f>
         <v>1.2500000000000001E-2</v>
@@ -3863,7 +3860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:9" x14ac:dyDescent="0.35">
       <c r="H52">
         <f t="shared" si="1"/>
         <v>2.5182573659027953E-2</v>
@@ -3872,7 +3869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:9" x14ac:dyDescent="0.35">
       <c r="H53">
         <f t="shared" si="1"/>
         <v>6.2956434147569884E-3</v>
@@ -3881,7 +3878,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.35">
       <c r="H54">
         <f t="shared" si="1"/>
         <v>3.1478217073784942E-3</v>
@@ -3891,7 +3888,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:9" x14ac:dyDescent="0.35">
       <c r="H55">
         <f t="shared" si="1"/>
         <v>2.5182573659027953E-3</v>
@@ -3900,7 +3897,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:9" x14ac:dyDescent="0.35">
       <c r="H56">
         <f t="shared" si="1"/>
         <v>1.2591286829513977E-3</v>
@@ -3934,165 +3931,165 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="98.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="98.453125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="12"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="13"/>
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>101</v>
       </c>
       <c r="B3" s="15"/>
     </row>
-    <row r="4" spans="1:2" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="82" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="50" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="50"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="17"/>
       <c r="B6" s="18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
       <c r="B7" s="18"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
       <c r="B8" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
       <c r="B9" s="20"/>
     </row>
-    <row r="10" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
       <c r="B10" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
       <c r="B11" s="18"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="18"/>
     </row>
-    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A14" s="16"/>
       <c r="B14" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="18"/>
     </row>
-    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="16"/>
       <c r="B16" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="16"/>
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="16"/>
       <c r="B19" s="18"/>
     </row>
-    <row r="20" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A20" s="16"/>
       <c r="B20" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="16"/>
       <c r="B21" s="20"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="23"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
     </row>
-    <row r="24" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="B24" s="25" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="52" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
       <c r="B26" s="25" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="24"/>
       <c r="B27" s="25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A28" s="24"/>
       <c r="B28" s="25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="24"/>
       <c r="B29" s="25" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="24"/>
       <c r="B30" s="25" t="s">
         <v>118</v>
@@ -4115,18 +4112,18 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="10"/>
+    <col min="1" max="1" width="8.7265625" style="10"/>
     <col min="2" max="2" width="20" style="10" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="10"/>
-    <col min="5" max="5" width="42.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="10" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="10"/>
+    <col min="3" max="3" width="23.1796875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="10"/>
+    <col min="5" max="5" width="42.453125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="26"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4143,7 +4140,7 @@
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -4158,7 +4155,7 @@
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="26"/>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -4173,7 +4170,7 @@
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -4198,7 +4195,7 @@
       <c r="J4" s="26"/>
       <c r="K4" s="26"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="28" t="s">
         <v>10</v>
       </c>
@@ -4219,7 +4216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="26"/>
       <c r="B6" s="29" t="s">
         <v>14</v>
@@ -4242,7 +4239,7 @@
       <c r="J6" s="26"/>
       <c r="K6" s="26"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="26"/>
       <c r="B7" s="31"/>
       <c r="C7" s="28" t="s">
@@ -4263,7 +4260,7 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="26"/>
       <c r="B8" s="31"/>
       <c r="C8" s="28" t="s">
@@ -4286,7 +4283,7 @@
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="26"/>
       <c r="B9" s="31"/>
       <c r="C9" s="28" t="s">
@@ -4313,7 +4310,7 @@
         <v>1068150020</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -4326,7 +4323,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="26"/>
       <c r="B11" s="29" t="s">
         <v>27</v>
@@ -4353,7 +4350,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="26"/>
       <c r="B12" s="31"/>
       <c r="C12" s="26"/>
@@ -4366,7 +4363,7 @@
       <c r="J12" s="26"/>
       <c r="K12" s="26"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="26"/>
       <c r="B13" s="29" t="s">
         <v>33</v>
@@ -4389,7 +4386,7 @@
       <c r="J13" s="26"/>
       <c r="K13" s="26"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="26"/>
       <c r="B14" s="31"/>
       <c r="C14" s="28" t="s">
@@ -4410,7 +4407,7 @@
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="26"/>
       <c r="B15" s="31"/>
       <c r="C15" s="28" t="s">
@@ -4433,7 +4430,7 @@
       <c r="J15" s="26"/>
       <c r="K15" s="26"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="26"/>
       <c r="B16" s="31"/>
       <c r="C16" s="28" t="s">
@@ -4460,7 +4457,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -4473,7 +4470,7 @@
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="26"/>
       <c r="B18" s="29" t="s">
         <v>47</v>
@@ -4496,7 +4493,7 @@
       <c r="J18" s="26"/>
       <c r="K18" s="26"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="26"/>
       <c r="B19" s="31"/>
       <c r="C19" s="28" t="s">
@@ -4517,7 +4514,7 @@
       <c r="J19" s="26"/>
       <c r="K19" s="26"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="26"/>
       <c r="B20" s="31"/>
       <c r="C20" s="33" t="s">
@@ -4538,7 +4535,7 @@
       <c r="J20" s="26"/>
       <c r="K20" s="26"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="26"/>
       <c r="B21" s="31"/>
       <c r="C21" s="28" t="s">
@@ -4559,7 +4556,7 @@
       <c r="J21" s="26"/>
       <c r="K21" s="26"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -4572,7 +4569,7 @@
       <c r="J22" s="26"/>
       <c r="K22" s="26"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -4585,7 +4582,7 @@
       <c r="J23" s="26"/>
       <c r="K23" s="26"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -4598,7 +4595,7 @@
       <c r="J24" s="26"/>
       <c r="K24" s="26"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="28" t="s">
         <v>56</v>
       </c>
@@ -4623,7 +4620,7 @@
       <c r="J25" s="26"/>
       <c r="K25" s="26"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="26"/>
       <c r="B26" s="31"/>
       <c r="C26" s="28" t="s">
@@ -4646,7 +4643,7 @@
       <c r="J26" s="26"/>
       <c r="K26" s="26"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="26"/>
       <c r="B27" s="31"/>
       <c r="C27" s="28" t="s">
@@ -4669,7 +4666,7 @@
       <c r="J27" s="26"/>
       <c r="K27" s="26"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="26"/>
       <c r="B28" s="31"/>
       <c r="C28" s="28" t="s">
@@ -4692,7 +4689,7 @@
       <c r="J28" s="26"/>
       <c r="K28" s="26"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="26"/>
       <c r="B29" s="31"/>
       <c r="C29" s="28" t="s">
@@ -4715,7 +4712,7 @@
       <c r="J29" s="26"/>
       <c r="K29" s="26"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="26"/>
       <c r="B30" s="31"/>
       <c r="C30" s="28" t="s">
@@ -4738,7 +4735,7 @@
       <c r="J30" s="26"/>
       <c r="K30" s="28"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="26"/>
       <c r="B31" s="31"/>
       <c r="C31" s="28" t="s">
@@ -4761,7 +4758,7 @@
       <c r="J31" s="26"/>
       <c r="K31" s="26"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="26"/>
       <c r="B32" s="31"/>
       <c r="C32" s="28" t="s">
@@ -4784,7 +4781,7 @@
       <c r="J32" s="26"/>
       <c r="K32" s="26"/>
     </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
@@ -4797,7 +4794,7 @@
       <c r="J33" s="26"/>
       <c r="K33" s="26"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="26"/>
       <c r="B34" s="29" t="s">
         <v>70</v>
@@ -4820,7 +4817,7 @@
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="26"/>
       <c r="B35" s="31"/>
       <c r="C35" s="28" t="s">
@@ -4841,7 +4838,7 @@
       <c r="J35" s="26"/>
       <c r="K35" s="26"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="26"/>
       <c r="B36" s="31"/>
       <c r="C36" s="28" t="s">
@@ -4862,7 +4859,7 @@
       <c r="J36" s="26"/>
       <c r="K36" s="26"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="26"/>
       <c r="B37" s="31"/>
       <c r="C37" s="28" t="s">
@@ -4883,7 +4880,7 @@
       <c r="J37" s="26"/>
       <c r="K37" s="26"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="26"/>
       <c r="B38" s="31"/>
       <c r="C38" s="28" t="s">
@@ -4904,7 +4901,7 @@
       <c r="J38" s="26"/>
       <c r="K38" s="26"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="26"/>
       <c r="B39" s="31"/>
       <c r="C39" s="28" t="s">
@@ -4925,7 +4922,7 @@
       <c r="J39" s="26"/>
       <c r="K39" s="26"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="26"/>
       <c r="B40" s="31"/>
       <c r="C40" s="28" t="s">
@@ -4946,7 +4943,7 @@
       <c r="J40" s="26"/>
       <c r="K40" s="26"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="26"/>
       <c r="B41" s="31"/>
       <c r="C41" s="28" t="s">
@@ -4967,7 +4964,7 @@
       <c r="J41" s="26"/>
       <c r="K41" s="26"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="26"/>
       <c r="B42" s="31"/>
       <c r="C42" s="28" t="s">
@@ -4988,7 +4985,7 @@
       <c r="J42" s="26"/>
       <c r="K42" s="26"/>
     </row>
-    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="26"/>
       <c r="B43" s="31"/>
       <c r="C43" s="28" t="s">
@@ -5022,22 +5019,22 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -5045,7 +5042,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -5119,7 +5116,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -5193,7 +5190,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -5267,7 +5264,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" s="46" t="s">
         <v>175</v>
       </c>
@@ -5341,7 +5338,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" s="46" t="s">
         <v>176</v>
       </c>
@@ -5415,7 +5412,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" s="46" t="s">
         <v>177</v>
       </c>
@@ -5489,7 +5486,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="46" t="s">
         <v>178</v>
       </c>
@@ -5563,7 +5560,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -5637,7 +5634,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -5711,7 +5708,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>181</v>
       </c>
@@ -5785,7 +5782,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>182</v>
       </c>
@@ -5859,7 +5856,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" s="46" t="s">
         <v>183</v>
       </c>
@@ -5933,7 +5930,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="46" t="s">
         <v>184</v>
       </c>
@@ -6007,7 +6004,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A17" s="46" t="s">
         <v>185</v>
       </c>
@@ -6081,7 +6078,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" s="46" t="s">
         <v>186</v>
       </c>
@@ -6155,7 +6152,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>187</v>
       </c>
@@ -6229,7 +6226,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>188</v>
       </c>
@@ -6303,7 +6300,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -6377,7 +6374,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>190</v>
       </c>
@@ -6451,7 +6448,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A23" s="46" t="s">
         <v>191</v>
       </c>
@@ -6525,7 +6522,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A24" s="46" t="s">
         <v>192</v>
       </c>
@@ -6599,7 +6596,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" s="46" t="s">
         <v>193</v>
       </c>
@@ -6673,7 +6670,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A26" s="46" t="s">
         <v>194</v>
       </c>
@@ -6747,7 +6744,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>195</v>
       </c>
@@ -6821,7 +6818,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>196</v>
       </c>
@@ -6895,7 +6892,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>197</v>
       </c>
@@ -6969,7 +6966,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>198</v>
       </c>
@@ -7043,7 +7040,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A31" s="46" t="s">
         <v>199</v>
       </c>
@@ -7117,7 +7114,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A32" s="46" t="s">
         <v>200</v>
       </c>
@@ -7191,7 +7188,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A33" s="46" t="s">
         <v>201</v>
       </c>
@@ -7265,7 +7262,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A34" s="46" t="s">
         <v>202</v>
       </c>
@@ -7339,7 +7336,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>203</v>
       </c>
@@ -7413,7 +7410,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>204</v>
       </c>
@@ -7487,7 +7484,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>205</v>
       </c>
@@ -7561,7 +7558,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>206</v>
       </c>
@@ -7635,7 +7632,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>207</v>
       </c>
@@ -7709,7 +7706,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>208</v>
       </c>
@@ -7783,7 +7780,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>213</v>
       </c>
@@ -7851,49 +7848,49 @@
         <v>735</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="L42" s="44"/>
       <c r="M42" s="44"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>753</v>
       </c>
       <c r="L43" s="44"/>
       <c r="M43" s="44"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>754</v>
       </c>
       <c r="L44" s="44"/>
       <c r="M44" s="44"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
       <c r="L45" s="44"/>
       <c r="M45" s="44"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="L46" s="44"/>
       <c r="M46" s="44"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
       <c r="L47" s="44"/>
       <c r="M47" s="44"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
       <c r="L48" s="44"/>
       <c r="M48" s="44"/>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="L49" s="44"/>
       <c r="M49" s="44"/>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="L50" s="44"/>
       <c r="M50" s="44"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>758</v>
       </c>
@@ -7903,7 +7900,7 @@
       <c r="L51" s="44"/>
       <c r="M51" s="44"/>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>214</v>
       </c>
@@ -7919,7 +7916,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>743</v>
       </c>
@@ -7993,7 +7990,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>174</v>
       </c>
@@ -8067,7 +8064,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>175</v>
       </c>
@@ -8132,7 +8129,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>176</v>
       </c>
@@ -8188,7 +8185,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>177</v>
       </c>
@@ -8244,7 +8241,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>178</v>
       </c>
@@ -8300,7 +8297,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -8353,7 +8350,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>180</v>
       </c>
@@ -8406,7 +8403,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>181</v>
       </c>
@@ -8459,7 +8456,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>182</v>
       </c>
@@ -8512,7 +8509,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>183</v>
       </c>
@@ -8565,7 +8562,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>184</v>
       </c>
@@ -8618,7 +8615,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>185</v>
       </c>
@@ -8671,7 +8668,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>186</v>
       </c>
@@ -8724,7 +8721,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -8777,7 +8774,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>188</v>
       </c>
@@ -8830,7 +8827,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>189</v>
       </c>
@@ -8883,7 +8880,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -8936,7 +8933,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>191</v>
       </c>
@@ -8989,7 +8986,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>192</v>
       </c>
@@ -9042,7 +9039,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>193</v>
       </c>
@@ -9095,7 +9092,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>194</v>
       </c>
@@ -9148,7 +9145,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>195</v>
       </c>
@@ -9201,7 +9198,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>196</v>
       </c>
@@ -9254,7 +9251,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>197</v>
       </c>
@@ -9307,7 +9304,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>198</v>
       </c>
@@ -9360,7 +9357,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>199</v>
       </c>
@@ -9416,7 +9413,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>200</v>
       </c>
@@ -9472,7 +9469,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>201</v>
       </c>
@@ -9528,7 +9525,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>202</v>
       </c>
@@ -9584,7 +9581,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>203</v>
       </c>
@@ -9640,7 +9637,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>204</v>
       </c>
@@ -9696,7 +9693,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>205</v>
       </c>
@@ -9752,7 +9749,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>206</v>
       </c>
@@ -9808,7 +9805,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>207</v>
       </c>
@@ -9873,7 +9870,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>208</v>
       </c>
@@ -9947,17 +9944,17 @@
         <v>735</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>757</v>
       </c>

</xml_diff>